<commit_message>
*results out of the oven*
</commit_message>
<xml_diff>
--- a/concerts/results/results.xlsx
+++ b/concerts/results/results.xlsx
@@ -572,7 +572,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -634,40 +645,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -676,52 +690,51 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+  <cellStyles count="34">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -747,6 +760,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Monthly taxi rides after big</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> concerts</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -755,100 +792,95 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet2!$H$7:$H$30</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>39813.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>39844.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>39872.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>39903.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>39933.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>39964.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>39994.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>40025.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>40056.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>40086.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>40117.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>40147.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0</c:v>
+                  <c:v>40178.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0</c:v>
+                  <c:v>40209.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0</c:v>
+                  <c:v>40237.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0</c:v>
+                  <c:v>40268.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.0</c:v>
+                  <c:v>40298.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0</c:v>
+                  <c:v>40329.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.0</c:v>
+                  <c:v>40359.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.0</c:v>
+                  <c:v>40390.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.0</c:v>
+                  <c:v>40421.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.0</c:v>
+                  <c:v>40451.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.0</c:v>
+                  <c:v>40482.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.0</c:v>
+                  <c:v>40512.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:invertIfNegative val="0"/>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$I$7:$I$30</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>669.0</c:v>
@@ -938,23 +970,23 @@
         <c:axId val="2096323288"/>
         <c:axId val="-2136626584"/>
       </c:barChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="2096323288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2136626584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="-2136626584"/>
         <c:scaling>
@@ -963,7 +995,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -972,11 +1004,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1003,6 +1030,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average taxi rides by concert</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1011,100 +1057,95 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet2!$H$32:$H$55</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>39813.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>39844.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>39872.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>39903.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>39933.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>39964.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>39994.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>40025.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>40056.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>40086.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>40117.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>40147.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0</c:v>
+                  <c:v>40178.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0</c:v>
+                  <c:v>40209.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0</c:v>
+                  <c:v>40237.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0</c:v>
+                  <c:v>40268.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.0</c:v>
+                  <c:v>40298.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0</c:v>
+                  <c:v>40329.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.0</c:v>
+                  <c:v>40359.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.0</c:v>
+                  <c:v>40390.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.0</c:v>
+                  <c:v>40421.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.0</c:v>
+                  <c:v>40451.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.0</c:v>
+                  <c:v>40482.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.0</c:v>
+                  <c:v>40512.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:invertIfNegative val="0"/>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$I$32:$I$55</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>669.0</c:v>
@@ -1194,23 +1235,23 @@
         <c:axId val="-2133317048"/>
         <c:axId val="-2133314072"/>
       </c:barChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="-2133317048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2133314072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="-2133314072"/>
         <c:scaling>
@@ -1219,7 +1260,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1228,11 +1269,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3261,8 +3297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3274,7 +3310,8 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="37.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
@@ -3447,277 +3484,277 @@
       <c r="E5" s="5">
         <v>27622</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>502.21818181818179</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>1</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>669</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>669</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="5">
         <v>5721</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>1144.2</v>
       </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="H7" s="11">
+        <v>39813</v>
+      </c>
+      <c r="I7" s="8">
         <v>669</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>3</v>
       </c>
       <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>3</v>
       </c>
       <c r="E8" s="5">
         <v>2153</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>538.25</v>
       </c>
-      <c r="H8" s="8">
-        <v>2</v>
-      </c>
-      <c r="I8" s="6">
+      <c r="H8" s="11">
+        <v>39844</v>
+      </c>
+      <c r="I8" s="8">
         <v>5721</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>4</v>
       </c>
       <c r="E9" s="5">
         <v>2404</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>801.33333333333337</v>
       </c>
-      <c r="H9" s="8">
-        <v>3</v>
-      </c>
-      <c r="I9" s="6">
+      <c r="H9" s="11">
+        <v>39872</v>
+      </c>
+      <c r="I9" s="8">
         <v>2153</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>5</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>5</v>
       </c>
       <c r="E10" s="5">
         <v>218</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>54.5</v>
       </c>
-      <c r="H10" s="8">
-        <v>4</v>
-      </c>
-      <c r="I10" s="6">
+      <c r="H10" s="11">
+        <v>39903</v>
+      </c>
+      <c r="I10" s="8">
         <v>2404</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>6</v>
       </c>
       <c r="B11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>6</v>
       </c>
       <c r="E11" s="5">
         <v>509</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>127.25</v>
       </c>
-      <c r="H11" s="8">
-        <v>5</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="H11" s="11">
+        <v>39933</v>
+      </c>
+      <c r="I11" s="8">
         <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>7</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>7</v>
       </c>
       <c r="E12" s="5">
         <v>757</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>378.5</v>
       </c>
-      <c r="H12" s="8">
-        <v>6</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="H12" s="11">
+        <v>39964</v>
+      </c>
+      <c r="I12" s="8">
         <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>8</v>
       </c>
       <c r="B13" s="5">
         <v>4</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>8</v>
       </c>
       <c r="E13" s="5">
         <v>1081</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>270.25</v>
       </c>
-      <c r="H13" s="8">
-        <v>7</v>
-      </c>
-      <c r="I13" s="6">
+      <c r="H13" s="11">
+        <v>39994</v>
+      </c>
+      <c r="I13" s="8">
         <v>757</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>9</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>9</v>
       </c>
       <c r="E14" s="5">
         <v>1111</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>277.75</v>
       </c>
-      <c r="H14" s="8">
-        <v>8</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="H14" s="11">
+        <v>40025</v>
+      </c>
+      <c r="I14" s="8">
         <v>1081</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>10</v>
       </c>
       <c r="B15" s="5">
         <v>5</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>10</v>
       </c>
       <c r="E15" s="5">
         <v>2337</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>467.4</v>
       </c>
-      <c r="H15" s="8">
-        <v>9</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="H15" s="11">
+        <v>40056</v>
+      </c>
+      <c r="I15" s="8">
         <v>1111</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>11</v>
       </c>
       <c r="B16" s="5">
         <v>10</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>11</v>
       </c>
       <c r="E16" s="5">
         <v>8839</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>883.9</v>
       </c>
-      <c r="H16" s="8">
-        <v>10</v>
-      </c>
-      <c r="I16" s="6">
+      <c r="H16" s="11">
+        <v>40086</v>
+      </c>
+      <c r="I16" s="8">
         <v>2337</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>12</v>
       </c>
       <c r="B17" s="5">
         <v>9</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>12</v>
       </c>
       <c r="E17" s="5">
         <v>1823</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>202.55555555555554</v>
       </c>
-      <c r="H17" s="8">
-        <v>11</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="11">
+        <v>40117</v>
+      </c>
+      <c r="I17" s="8">
         <v>8839</v>
       </c>
     </row>
@@ -3734,266 +3771,266 @@
       <c r="E18" s="5">
         <v>35179</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>639.61818181818182</v>
       </c>
-      <c r="H18" s="8">
-        <v>12</v>
-      </c>
-      <c r="I18" s="6">
+      <c r="H18" s="11">
+        <v>40147</v>
+      </c>
+      <c r="I18" s="8">
         <v>1823</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>2</v>
       </c>
       <c r="B19" s="5">
         <v>5</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
       <c r="E19" s="5">
         <v>6365</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>1273</v>
       </c>
       <c r="H19" s="11">
-        <v>1</v>
-      </c>
-      <c r="I19" s="12">
+        <v>40178</v>
+      </c>
+      <c r="I19" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>3</v>
       </c>
       <c r="B20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>3</v>
       </c>
       <c r="E20" s="5">
         <v>2726</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>908.66666666666663</v>
       </c>
-      <c r="H20" s="8">
-        <v>2</v>
-      </c>
-      <c r="I20" s="6">
+      <c r="H20" s="11">
+        <v>40209</v>
+      </c>
+      <c r="I20" s="8">
         <v>6365</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>4</v>
       </c>
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>4</v>
       </c>
       <c r="E21" s="5">
         <v>4170</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>834</v>
       </c>
-      <c r="H21" s="8">
-        <v>3</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="H21" s="11">
+        <v>40237</v>
+      </c>
+      <c r="I21" s="8">
         <v>2726</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>5</v>
       </c>
       <c r="B22" s="5">
         <v>4</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>5</v>
       </c>
       <c r="E22" s="5">
         <v>2833</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>708.25</v>
       </c>
-      <c r="H22" s="8">
-        <v>4</v>
-      </c>
-      <c r="I22" s="6">
+      <c r="H22" s="11">
+        <v>40268</v>
+      </c>
+      <c r="I22" s="8">
         <v>4170</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>6</v>
       </c>
       <c r="B23" s="5">
         <v>2</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>6</v>
       </c>
       <c r="E23" s="5">
         <v>87</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>43.5</v>
       </c>
-      <c r="H23" s="8">
-        <v>5</v>
-      </c>
-      <c r="I23" s="6">
+      <c r="H23" s="11">
+        <v>40298</v>
+      </c>
+      <c r="I23" s="8">
         <v>2833</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>7</v>
       </c>
       <c r="B24" s="5">
         <v>7</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>7</v>
       </c>
       <c r="E24" s="5">
         <v>5001</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>714.42857142857144</v>
       </c>
-      <c r="H24" s="8">
-        <v>6</v>
-      </c>
-      <c r="I24" s="6">
+      <c r="H24" s="11">
+        <v>40329</v>
+      </c>
+      <c r="I24" s="8">
         <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>8</v>
       </c>
       <c r="B25" s="5">
         <v>2</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>8</v>
       </c>
       <c r="E25" s="5">
         <v>2139</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>1069.5</v>
       </c>
-      <c r="H25" s="8">
-        <v>7</v>
-      </c>
-      <c r="I25" s="6">
+      <c r="H25" s="11">
+        <v>40359</v>
+      </c>
+      <c r="I25" s="8">
         <v>5001</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>9</v>
       </c>
       <c r="B26" s="5">
         <v>11</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>9</v>
       </c>
       <c r="E26" s="5">
         <v>4783</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>434.81818181818181</v>
       </c>
-      <c r="H26" s="8">
-        <v>8</v>
-      </c>
-      <c r="I26" s="6">
+      <c r="H26" s="11">
+        <v>40390</v>
+      </c>
+      <c r="I26" s="8">
         <v>2139</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>10</v>
       </c>
       <c r="B27" s="5">
         <v>3</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>10</v>
       </c>
       <c r="E27" s="5">
         <v>1395</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="7">
         <v>465</v>
       </c>
-      <c r="H27" s="8">
-        <v>9</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="H27" s="11">
+        <v>40421</v>
+      </c>
+      <c r="I27" s="8">
         <v>4783</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>11</v>
       </c>
       <c r="B28" s="5">
         <v>2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>11</v>
       </c>
       <c r="E28" s="5">
         <v>815</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="7">
         <v>407.5</v>
       </c>
-      <c r="H28" s="8">
-        <v>10</v>
-      </c>
-      <c r="I28" s="6">
+      <c r="H28" s="11">
+        <v>40451</v>
+      </c>
+      <c r="I28" s="8">
         <v>1395</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>12</v>
       </c>
       <c r="B29" s="5">
         <v>11</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>12</v>
       </c>
       <c r="E29" s="5">
         <v>4865</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>442.27272727272725</v>
       </c>
-      <c r="H29" s="8">
-        <v>11</v>
-      </c>
-      <c r="I29" s="6">
+      <c r="H29" s="11">
+        <v>40482</v>
+      </c>
+      <c r="I29" s="8">
         <v>815</v>
       </c>
     </row>
@@ -4010,205 +4047,208 @@
       <c r="E30" s="5">
         <v>62801</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="7">
         <v>570.91818181818178</v>
       </c>
-      <c r="H30" s="8">
-        <v>12</v>
-      </c>
-      <c r="I30" s="6">
+      <c r="H30" s="11">
+        <v>40512</v>
+      </c>
+      <c r="I30" s="8">
         <v>4865</v>
       </c>
     </row>
+    <row r="31" spans="1:9">
+      <c r="I31" s="10"/>
+    </row>
     <row r="32" spans="1:9">
-      <c r="H32" s="8">
-        <v>1</v>
-      </c>
-      <c r="I32" s="10">
+      <c r="H32" s="11">
+        <v>39813</v>
+      </c>
+      <c r="I32" s="8">
         <v>669</v>
       </c>
     </row>
     <row r="33" spans="8:9">
-      <c r="H33" s="8">
-        <v>2</v>
-      </c>
-      <c r="I33" s="10">
+      <c r="H33" s="11">
+        <v>39844</v>
+      </c>
+      <c r="I33" s="8">
         <v>1144.2</v>
       </c>
     </row>
     <row r="34" spans="8:9">
-      <c r="H34" s="8">
-        <v>3</v>
-      </c>
-      <c r="I34" s="10">
+      <c r="H34" s="11">
+        <v>39872</v>
+      </c>
+      <c r="I34" s="8">
         <v>538.25</v>
       </c>
     </row>
     <row r="35" spans="8:9">
-      <c r="H35" s="8">
-        <v>4</v>
-      </c>
-      <c r="I35" s="10">
+      <c r="H35" s="11">
+        <v>39903</v>
+      </c>
+      <c r="I35" s="8">
         <v>801.33333333333337</v>
       </c>
     </row>
     <row r="36" spans="8:9">
-      <c r="H36" s="8">
-        <v>5</v>
-      </c>
-      <c r="I36" s="10">
+      <c r="H36" s="11">
+        <v>39933</v>
+      </c>
+      <c r="I36" s="8">
         <v>54.5</v>
       </c>
     </row>
     <row r="37" spans="8:9">
-      <c r="H37" s="8">
-        <v>6</v>
-      </c>
-      <c r="I37" s="10">
+      <c r="H37" s="11">
+        <v>39964</v>
+      </c>
+      <c r="I37" s="8">
         <v>127.25</v>
       </c>
     </row>
     <row r="38" spans="8:9">
-      <c r="H38" s="8">
-        <v>7</v>
-      </c>
-      <c r="I38" s="10">
+      <c r="H38" s="11">
+        <v>39994</v>
+      </c>
+      <c r="I38" s="8">
         <v>378.5</v>
       </c>
     </row>
     <row r="39" spans="8:9">
-      <c r="H39" s="8">
-        <v>8</v>
-      </c>
-      <c r="I39" s="10">
+      <c r="H39" s="11">
+        <v>40025</v>
+      </c>
+      <c r="I39" s="8">
         <v>270.25</v>
       </c>
     </row>
     <row r="40" spans="8:9">
-      <c r="H40" s="8">
-        <v>9</v>
-      </c>
-      <c r="I40" s="10">
+      <c r="H40" s="11">
+        <v>40056</v>
+      </c>
+      <c r="I40" s="8">
         <v>277.75</v>
       </c>
     </row>
     <row r="41" spans="8:9">
-      <c r="H41" s="8">
-        <v>10</v>
-      </c>
-      <c r="I41" s="10">
+      <c r="H41" s="11">
+        <v>40086</v>
+      </c>
+      <c r="I41" s="8">
         <v>467.4</v>
       </c>
     </row>
     <row r="42" spans="8:9">
-      <c r="H42" s="8">
-        <v>11</v>
-      </c>
-      <c r="I42" s="10">
+      <c r="H42" s="11">
+        <v>40117</v>
+      </c>
+      <c r="I42" s="8">
         <v>883.9</v>
       </c>
     </row>
     <row r="43" spans="8:9">
-      <c r="H43" s="8">
-        <v>12</v>
-      </c>
-      <c r="I43" s="10">
+      <c r="H43" s="11">
+        <v>40147</v>
+      </c>
+      <c r="I43" s="8">
         <v>202.55555555555554</v>
       </c>
     </row>
     <row r="44" spans="8:9">
       <c r="H44" s="11">
-        <v>1</v>
-      </c>
-      <c r="I44" s="13">
+        <v>40178</v>
+      </c>
+      <c r="I44" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="8:9">
-      <c r="H45" s="8">
-        <v>2</v>
-      </c>
-      <c r="I45" s="10">
+      <c r="H45" s="11">
+        <v>40209</v>
+      </c>
+      <c r="I45" s="8">
         <v>1273</v>
       </c>
     </row>
     <row r="46" spans="8:9">
-      <c r="H46" s="8">
-        <v>3</v>
-      </c>
-      <c r="I46" s="10">
+      <c r="H46" s="11">
+        <v>40237</v>
+      </c>
+      <c r="I46" s="8">
         <v>908.66666666666663</v>
       </c>
     </row>
     <row r="47" spans="8:9">
-      <c r="H47" s="8">
-        <v>4</v>
-      </c>
-      <c r="I47" s="10">
+      <c r="H47" s="11">
+        <v>40268</v>
+      </c>
+      <c r="I47" s="8">
         <v>834</v>
       </c>
     </row>
     <row r="48" spans="8:9">
-      <c r="H48" s="8">
-        <v>5</v>
-      </c>
-      <c r="I48" s="10">
+      <c r="H48" s="11">
+        <v>40298</v>
+      </c>
+      <c r="I48" s="8">
         <v>708.25</v>
       </c>
     </row>
     <row r="49" spans="8:9">
-      <c r="H49" s="8">
-        <v>6</v>
-      </c>
-      <c r="I49" s="10">
+      <c r="H49" s="11">
+        <v>40329</v>
+      </c>
+      <c r="I49" s="8">
         <v>43.5</v>
       </c>
     </row>
     <row r="50" spans="8:9">
-      <c r="H50" s="8">
-        <v>7</v>
-      </c>
-      <c r="I50" s="10">
+      <c r="H50" s="11">
+        <v>40359</v>
+      </c>
+      <c r="I50" s="8">
         <v>714.42857142857144</v>
       </c>
     </row>
     <row r="51" spans="8:9">
-      <c r="H51" s="8">
-        <v>8</v>
-      </c>
-      <c r="I51" s="10">
+      <c r="H51" s="11">
+        <v>40390</v>
+      </c>
+      <c r="I51" s="8">
         <v>1069.5</v>
       </c>
     </row>
     <row r="52" spans="8:9">
-      <c r="H52" s="8">
-        <v>9</v>
-      </c>
-      <c r="I52" s="10">
+      <c r="H52" s="11">
+        <v>40421</v>
+      </c>
+      <c r="I52" s="8">
         <v>434.81818181818181</v>
       </c>
     </row>
     <row r="53" spans="8:9">
-      <c r="H53" s="8">
-        <v>10</v>
-      </c>
-      <c r="I53" s="10">
+      <c r="H53" s="11">
+        <v>40451</v>
+      </c>
+      <c r="I53" s="8">
         <v>465</v>
       </c>
     </row>
     <row r="54" spans="8:9">
-      <c r="H54" s="8">
-        <v>11</v>
-      </c>
-      <c r="I54" s="10">
+      <c r="H54" s="11">
+        <v>40482</v>
+      </c>
+      <c r="I54" s="8">
         <v>407.5</v>
       </c>
     </row>
     <row r="55" spans="8:9">
-      <c r="H55" s="8">
-        <v>12</v>
-      </c>
-      <c r="I55" s="10">
+      <c r="H55" s="11">
+        <v>40512</v>
+      </c>
+      <c r="I55" s="8">
         <v>442.27272727272725</v>
       </c>
     </row>

</xml_diff>